<commit_message>
Se agregan modulos para verificacion
</commit_message>
<xml_diff>
--- a/documentation/test_plan.xlsx
+++ b/documentation/test_plan.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="87">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="88">
   <si>
     <t xml:space="preserve">PLAN DE PRUEBAS</t>
   </si>
@@ -77,6 +77,9 @@
   </si>
   <si>
     <t xml:space="preserve">COMENTARIOS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TEST CASE</t>
   </si>
   <si>
     <t xml:space="preserve">T_NORMAL_B</t>
@@ -295,7 +298,6 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
-      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -313,7 +315,7 @@
       <family val="0"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -340,8 +342,14 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FF729FCF"/>
-        <bgColor rgb="FF969696"/>
+        <fgColor rgb="FF2A6099"/>
+        <bgColor rgb="FF666699"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFDEE6EF"/>
+        <bgColor rgb="FFCCFFFF"/>
       </patternFill>
     </fill>
   </fills>
@@ -379,7 +387,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="14">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -422,6 +430,14 @@
     </xf>
     <xf numFmtId="164" fontId="0" fillId="5" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="6" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
@@ -455,13 +471,13 @@
       <rgbColor rgb="FF008080"/>
       <rgbColor rgb="FFB3CAC7"/>
       <rgbColor rgb="FF808080"/>
-      <rgbColor rgb="FF729FCF"/>
+      <rgbColor rgb="FF9999FF"/>
       <rgbColor rgb="FF993366"/>
       <rgbColor rgb="FFFFFFCC"/>
-      <rgbColor rgb="FFCCFFFF"/>
+      <rgbColor rgb="FFDEE6EF"/>
       <rgbColor rgb="FF660066"/>
       <rgbColor rgb="FFFF8080"/>
-      <rgbColor rgb="FF0066CC"/>
+      <rgbColor rgb="FF2A6099"/>
       <rgbColor rgb="FFCCCCFF"/>
       <rgbColor rgb="FF000080"/>
       <rgbColor rgb="FFFF00FF"/>
@@ -611,470 +627,493 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:H27"/>
+  <dimension ref="A1:I27"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="86" zoomScaleNormal="86" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B27" activeCellId="0" sqref="B27"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="98" zoomScaleNormal="98" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D32" activeCellId="0" sqref="D32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="5.32"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="20.17"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="51.49"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="36.56"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="37.05"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="20.17"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="16.27"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="19.2"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="22.31"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="7.89"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="23.68"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="51.49"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="39.85"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="37.05"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="24.56"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="16.27"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="1" width="19.2"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="2" t="s">
+      <c r="B1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2"/>
       <c r="C1" s="2"/>
       <c r="D1" s="2"/>
       <c r="E1" s="2"/>
       <c r="F1" s="2"/>
+      <c r="G1" s="2"/>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="2"/>
-      <c r="B2" s="3"/>
+      <c r="B2" s="2"/>
       <c r="C2" s="3"/>
       <c r="D2" s="3"/>
       <c r="E2" s="3"/>
       <c r="F2" s="3"/>
+      <c r="G2" s="3"/>
     </row>
     <row r="3" customFormat="false" ht="17.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C3" s="4" t="s">
+      <c r="D3" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="D3" s="5" t="s">
+      <c r="E3" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="E3" s="1" t="s">
+      <c r="F3" s="1" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="17.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C4" s="4"/>
-      <c r="D4" s="5" t="s">
+      <c r="D4" s="4"/>
+      <c r="E4" s="5" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="17.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C5" s="6" t="s">
+      <c r="D5" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="D5" s="7" t="s">
+      <c r="E5" s="7" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="17.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C6" s="6"/>
-      <c r="D6" s="7" t="s">
+      <c r="D6" s="6"/>
+      <c r="E6" s="7" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="17.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C7" s="8" t="s">
+      <c r="D7" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="D7" s="9" t="s">
+      <c r="E7" s="9" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="17.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C8" s="8"/>
-      <c r="D8" s="9" t="s">
+      <c r="D8" s="8"/>
+      <c r="E8" s="9" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="10" t="s">
+      <c r="A9" s="10"/>
+      <c r="B9" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="B9" s="10" t="s">
+      <c r="C9" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="C9" s="10" t="s">
+      <c r="D9" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="D9" s="10" t="s">
+      <c r="E9" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="E9" s="10" t="s">
+      <c r="F9" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="F9" s="10" t="s">
+      <c r="G9" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="G9" s="10" t="s">
+      <c r="H9" s="10" t="s">
         <v>17</v>
       </c>
-      <c r="H9" s="10" t="s">
+      <c r="I9" s="10" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="10" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="1" t="n">
+    <row r="10" customFormat="false" ht="23.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A10" s="11" t="s">
+        <v>19</v>
+      </c>
+      <c r="B10" s="12" t="n">
         <v>1</v>
       </c>
-      <c r="B10" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="C10" s="1" t="s">
+      <c r="C10" s="12" t="s">
         <v>20</v>
       </c>
       <c r="D10" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="E10" s="11" t="s">
+      <c r="E10" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="F10" s="11" t="s">
+      <c r="F10" s="13" t="s">
         <v>23</v>
       </c>
+      <c r="G10" s="13" t="s">
+        <v>24</v>
+      </c>
     </row>
     <row r="11" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="1" t="n">
+      <c r="A11" s="11"/>
+      <c r="B11" s="12" t="n">
         <v>2</v>
       </c>
-      <c r="B11" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="C11" s="1" t="s">
+      <c r="C11" s="12" t="s">
         <v>25</v>
       </c>
       <c r="D11" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="E11" s="11" t="s">
-        <v>22</v>
-      </c>
-      <c r="F11" s="1" t="s">
+      <c r="E11" s="1" t="s">
         <v>27</v>
       </c>
+      <c r="F11" s="13" t="s">
+        <v>23</v>
+      </c>
+      <c r="G11" s="1" t="s">
+        <v>28</v>
+      </c>
     </row>
     <row r="12" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="1" t="n">
+      <c r="A12" s="11"/>
+      <c r="B12" s="12" t="n">
         <v>3</v>
       </c>
-      <c r="B12" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="C12" s="1" t="s">
+      <c r="C12" s="12" t="s">
         <v>29</v>
       </c>
       <c r="D12" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="E12" s="11" t="s">
+      <c r="E12" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="F12" s="11" t="s">
-        <v>23</v>
+      <c r="F12" s="13" t="s">
+        <v>32</v>
+      </c>
+      <c r="G12" s="13" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="1" t="n">
+      <c r="A13" s="11"/>
+      <c r="B13" s="12" t="n">
         <v>4</v>
       </c>
-      <c r="B13" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="C13" s="1" t="s">
+      <c r="C13" s="12" t="s">
         <v>33</v>
       </c>
       <c r="D13" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="E13" s="11" t="s">
+      <c r="E13" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="F13" s="11" t="s">
-        <v>23</v>
+      <c r="F13" s="13" t="s">
+        <v>36</v>
+      </c>
+      <c r="G13" s="13" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="1" t="n">
+      <c r="A14" s="11"/>
+      <c r="B14" s="12" t="n">
         <v>5</v>
       </c>
-      <c r="B14" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="C14" s="1" t="s">
+      <c r="C14" s="12" t="s">
         <v>37</v>
       </c>
       <c r="D14" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="E14" s="11" t="s">
+      <c r="E14" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="F14" s="1" t="s">
+      <c r="F14" s="13" t="s">
         <v>40</v>
       </c>
+      <c r="G14" s="1" t="s">
+        <v>41</v>
+      </c>
     </row>
     <row r="15" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="1" t="n">
+      <c r="A15" s="11"/>
+      <c r="B15" s="12" t="n">
         <v>6</v>
       </c>
-      <c r="B15" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="C15" s="1" t="s">
+      <c r="C15" s="12" t="s">
         <v>42</v>
       </c>
       <c r="D15" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="E15" s="11" t="s">
+      <c r="E15" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="F15" s="1" t="s">
-        <v>40</v>
+      <c r="F15" s="13" t="s">
+        <v>45</v>
+      </c>
+      <c r="G15" s="1" t="s">
+        <v>41</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="1" t="n">
+      <c r="A16" s="11"/>
+      <c r="B16" s="12" t="n">
         <v>7</v>
       </c>
-      <c r="B16" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="C16" s="1" t="s">
+      <c r="C16" s="12" t="s">
         <v>46</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="E16" s="11" t="s">
+        <v>47</v>
+      </c>
+      <c r="E16" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="F16" s="1" t="s">
-        <v>47</v>
+      <c r="F16" s="13" t="s">
+        <v>32</v>
+      </c>
+      <c r="G16" s="1" t="s">
+        <v>48</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="1" t="n">
+      <c r="A17" s="11"/>
+      <c r="B17" s="12" t="n">
         <v>8</v>
       </c>
-      <c r="B17" s="1" t="s">
+      <c r="C17" s="12" t="s">
+        <v>49</v>
+      </c>
+      <c r="D17" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="E17" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="F17" s="13" t="s">
+        <v>36</v>
+      </c>
+      <c r="G17" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="C17" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="D17" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="E17" s="11" t="s">
-        <v>35</v>
-      </c>
-      <c r="F17" s="1" t="s">
-        <v>47</v>
-      </c>
     </row>
     <row r="18" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="1" t="n">
+      <c r="A18" s="11"/>
+      <c r="B18" s="12" t="n">
         <v>9</v>
       </c>
-      <c r="B18" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="C18" s="1" t="s">
+      <c r="C18" s="12" t="s">
         <v>51</v>
       </c>
       <c r="D18" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="E18" s="11" t="s">
-        <v>22</v>
-      </c>
-      <c r="F18" s="11" t="s">
+      <c r="E18" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="F18" s="13" t="s">
         <v>23</v>
       </c>
+      <c r="G18" s="13" t="s">
+        <v>24</v>
+      </c>
     </row>
     <row r="19" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="1" t="n">
+      <c r="A19" s="11"/>
+      <c r="B19" s="12" t="n">
         <v>10</v>
       </c>
-      <c r="B19" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="C19" s="1" t="s">
+      <c r="C19" s="12" t="s">
         <v>54</v>
       </c>
       <c r="D19" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="E19" s="11" t="s">
-        <v>22</v>
-      </c>
-      <c r="F19" s="1" t="s">
+      <c r="E19" s="1" t="s">
         <v>56</v>
       </c>
+      <c r="F19" s="13" t="s">
+        <v>23</v>
+      </c>
+      <c r="G19" s="1" t="s">
+        <v>57</v>
+      </c>
     </row>
     <row r="20" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="1" t="n">
+      <c r="A20" s="11"/>
+      <c r="B20" s="12" t="n">
         <v>12</v>
       </c>
-      <c r="B20" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="C20" s="1" t="s">
+      <c r="C20" s="12" t="s">
         <v>58</v>
       </c>
       <c r="D20" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="E20" s="11" t="s">
+      <c r="E20" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="F20" s="1" t="s">
+      <c r="F20" s="13" t="s">
         <v>61</v>
       </c>
+      <c r="G20" s="1" t="s">
+        <v>62</v>
+      </c>
     </row>
     <row r="21" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="1" t="n">
+      <c r="A21" s="11"/>
+      <c r="B21" s="12" t="n">
         <v>13</v>
       </c>
-      <c r="B21" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="C21" s="1" t="s">
+      <c r="C21" s="12" t="s">
         <v>63</v>
       </c>
       <c r="D21" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="E21" s="11" t="s">
+      <c r="E21" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="F21" s="1" t="s">
-        <v>61</v>
+      <c r="F21" s="13" t="s">
+        <v>66</v>
+      </c>
+      <c r="G21" s="1" t="s">
+        <v>62</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="1" t="n">
+      <c r="A22" s="11"/>
+      <c r="B22" s="12" t="n">
         <v>14</v>
       </c>
-      <c r="B22" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="C22" s="1" t="s">
+      <c r="C22" s="12" t="s">
         <v>67</v>
       </c>
       <c r="D22" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="E22" s="11" t="s">
+      <c r="E22" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="F22" s="11" t="s">
-        <v>23</v>
+      <c r="F22" s="13" t="s">
+        <v>70</v>
+      </c>
+      <c r="G22" s="13" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="23.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="1" t="n">
+      <c r="A23" s="11"/>
+      <c r="B23" s="12" t="n">
         <v>15</v>
       </c>
-      <c r="B23" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="C23" s="1" t="s">
+      <c r="C23" s="12" t="s">
         <v>71</v>
       </c>
       <c r="D23" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="E23" s="11" t="s">
-        <v>35</v>
-      </c>
-      <c r="F23" s="1" t="s">
+      <c r="E23" s="1" t="s">
         <v>73</v>
       </c>
+      <c r="F23" s="13" t="s">
+        <v>36</v>
+      </c>
+      <c r="G23" s="1" t="s">
+        <v>74</v>
+      </c>
     </row>
     <row r="24" customFormat="false" ht="23.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="1" t="n">
+      <c r="A24" s="11"/>
+      <c r="B24" s="12" t="n">
         <v>16</v>
       </c>
-      <c r="B24" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="C24" s="1" t="s">
+      <c r="C24" s="12" t="s">
         <v>75</v>
       </c>
       <c r="D24" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="E24" s="11" t="s">
-        <v>31</v>
-      </c>
-      <c r="F24" s="1" t="s">
-        <v>73</v>
+      <c r="E24" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="F24" s="13" t="s">
+        <v>32</v>
+      </c>
+      <c r="G24" s="1" t="s">
+        <v>74</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="23.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="1" t="n">
+      <c r="A25" s="11"/>
+      <c r="B25" s="12" t="n">
         <v>17</v>
       </c>
-      <c r="B25" s="1" t="s">
-        <v>77</v>
-      </c>
-      <c r="C25" s="1" t="s">
+      <c r="C25" s="12" t="s">
         <v>78</v>
       </c>
-      <c r="D25" s="11" t="s">
+      <c r="D25" s="1" t="s">
         <v>79</v>
       </c>
-      <c r="E25" s="11" t="s">
+      <c r="E25" s="13" t="s">
         <v>80</v>
       </c>
-      <c r="F25" s="11" t="s">
-        <v>23</v>
+      <c r="F25" s="13" t="s">
+        <v>81</v>
+      </c>
+      <c r="G25" s="13" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="23.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="1" t="n">
+      <c r="A26" s="11"/>
+      <c r="B26" s="12" t="n">
         <v>19</v>
       </c>
-      <c r="B26" s="1" t="s">
-        <v>81</v>
-      </c>
-      <c r="C26" s="1" t="s">
+      <c r="C26" s="12" t="s">
         <v>82</v>
       </c>
       <c r="D26" s="1" t="s">
         <v>83</v>
       </c>
-      <c r="E26" s="11" t="s">
-        <v>22</v>
+      <c r="E26" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="F26" s="13" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="1" t="n">
+      <c r="A27" s="11"/>
+      <c r="B27" s="12" t="n">
         <v>20</v>
       </c>
-      <c r="B27" s="1" t="s">
-        <v>84</v>
-      </c>
-      <c r="C27" s="1" t="s">
+      <c r="C27" s="12" t="s">
         <v>85</v>
       </c>
       <c r="D27" s="1" t="s">
         <v>86</v>
       </c>
+      <c r="E27" s="1" t="s">
+        <v>87</v>
+      </c>
     </row>
   </sheetData>
-  <mergeCells count="4">
-    <mergeCell ref="A1:F1"/>
-    <mergeCell ref="C3:C4"/>
-    <mergeCell ref="C5:C6"/>
-    <mergeCell ref="C7:C8"/>
+  <mergeCells count="5">
+    <mergeCell ref="B1:G1"/>
+    <mergeCell ref="D3:D4"/>
+    <mergeCell ref="D5:D6"/>
+    <mergeCell ref="D7:D8"/>
+    <mergeCell ref="A10:A27"/>
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>

</xml_diff>